<commit_message>
Signed-off-by: Enrique Alvarez Villace <enrique.alvarez.villace@gmail.com>
</commit_message>
<xml_diff>
--- a/coronavirus/Datos.xlsx
+++ b/coronavirus/Datos.xlsx
@@ -353,7 +353,7 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D2" sqref="D2:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,6 +416,12 @@
         <f t="shared" ref="B4:B41" si="1">B3+"4:00:00"</f>
         <v>44324.666666666664</v>
       </c>
+      <c r="C4">
+        <v>34</v>
+      </c>
+      <c r="D4">
+        <v>98</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -426,6 +432,12 @@
         <f t="shared" si="1"/>
         <v>44324.833333333328</v>
       </c>
+      <c r="C5">
+        <v>33</v>
+      </c>
+      <c r="D5">
+        <v>99</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -436,6 +448,12 @@
         <f t="shared" si="1"/>
         <v>44324.999999999993</v>
       </c>
+      <c r="C6">
+        <v>32</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -446,6 +464,12 @@
         <f t="shared" si="1"/>
         <v>44325.166666666657</v>
       </c>
+      <c r="C7">
+        <v>31</v>
+      </c>
+      <c r="D7">
+        <v>101</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -456,6 +480,12 @@
         <f t="shared" si="1"/>
         <v>44325.333333333321</v>
       </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>102</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -466,6 +496,12 @@
         <f t="shared" si="1"/>
         <v>44325.499999999985</v>
       </c>
+      <c r="C9">
+        <v>29</v>
+      </c>
+      <c r="D9">
+        <v>103</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -476,6 +512,12 @@
         <f t="shared" si="1"/>
         <v>44325.66666666665</v>
       </c>
+      <c r="C10">
+        <v>28</v>
+      </c>
+      <c r="D10">
+        <v>104</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -486,6 +528,12 @@
         <f t="shared" si="1"/>
         <v>44325.833333333314</v>
       </c>
+      <c r="C11">
+        <v>27</v>
+      </c>
+      <c r="D11">
+        <v>105</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -496,6 +544,12 @@
         <f t="shared" si="1"/>
         <v>44325.999999999978</v>
       </c>
+      <c r="C12">
+        <v>26</v>
+      </c>
+      <c r="D12">
+        <v>106</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -506,6 +560,12 @@
         <f t="shared" si="1"/>
         <v>44326.166666666642</v>
       </c>
+      <c r="C13">
+        <v>25</v>
+      </c>
+      <c r="D13">
+        <v>107</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -516,6 +576,12 @@
         <f t="shared" si="1"/>
         <v>44326.333333333307</v>
       </c>
+      <c r="C14">
+        <v>24</v>
+      </c>
+      <c r="D14">
+        <v>108</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -525,6 +591,12 @@
       <c r="B15" s="2">
         <f t="shared" si="1"/>
         <v>44326.499999999971</v>
+      </c>
+      <c r="C15">
+        <v>23</v>
+      </c>
+      <c r="D15">
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>